<commit_message>
time of front added
</commit_message>
<xml_diff>
--- a/Mehdi.xlsx
+++ b/Mehdi.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BioDroid\Desktop\schedule git\Schedule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\schedule git\Schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="23040" windowHeight="9180"/>
+    <workbookView xWindow="0" yWindow="4200" windowWidth="23040" windowHeight="9180"/>
   </bookViews>
   <sheets>
     <sheet name="Scheduling" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="86">
   <si>
     <t>Visual Studio Code</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>portofilo</t>
+  </si>
+  <si>
+    <t>Front</t>
   </si>
 </sst>
 </file>
@@ -656,7 +659,7 @@
                   <c:v>370</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1911,8 +1914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG269"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2084,167 +2087,172 @@
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>13</v>
+      <c r="A10" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" s="3">
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
@@ -3183,7 +3191,7 @@
       </c>
       <c r="F2">
         <f>SUM(Scheduling!G:G,Scheduling!G1)</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G2">
         <f>SUM(Scheduling!H:H,Scheduling!H1)</f>

</xml_diff>